<commit_message>
Updated for 03/05; updated rolling mean window to 7 days to smooth out the weekend effect
</commit_message>
<xml_diff>
--- a/corona_scotland.xlsx
+++ b/corona_scotland.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="33">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -273,10 +273,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F758"/>
+  <dimension ref="A1:F773"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A747" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C771" activeCellId="0" sqref="C771"/>
+      <selection pane="topLeft" activeCell="F759" activeCellId="0" sqref="F759"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7434,7 +7434,7 @@
       <c r="E728" s="5"/>
     </row>
     <row r="729" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A729" s="6" t="n">
+      <c r="A729" s="3" t="n">
         <v>43952</v>
       </c>
       <c r="B729" s="5" t="s">
@@ -7594,7 +7594,7 @@
       <c r="E743" s="5"/>
     </row>
     <row r="744" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A744" s="6" t="n">
+      <c r="A744" s="3" t="n">
         <v>43953</v>
       </c>
       <c r="B744" s="5" t="s">
@@ -7752,6 +7752,166 @@
       </c>
       <c r="D758" s="5"/>
       <c r="E758" s="5"/>
+    </row>
+    <row r="759" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A759" s="6" t="n">
+        <v>43954</v>
+      </c>
+      <c r="B759" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C759" s="5" t="n">
+        <v>799</v>
+      </c>
+      <c r="D759" s="5" t="n">
+        <v>60295</v>
+      </c>
+      <c r="E759" s="5" t="n">
+        <v>12097</v>
+      </c>
+      <c r="F759" s="5" t="n">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="760" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B760" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C760" s="5" t="n">
+        <v>284</v>
+      </c>
+      <c r="D760" s="5"/>
+      <c r="E760" s="5"/>
+    </row>
+    <row r="761" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B761" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C761" s="5" t="n">
+        <v>250</v>
+      </c>
+      <c r="D761" s="5"/>
+      <c r="E761" s="5"/>
+    </row>
+    <row r="762" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B762" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C762" s="5" t="n">
+        <v>776</v>
+      </c>
+      <c r="D762" s="5"/>
+      <c r="E762" s="5"/>
+    </row>
+    <row r="763" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B763" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C763" s="5" t="n">
+        <v>788</v>
+      </c>
+      <c r="D763" s="5"/>
+      <c r="E763" s="5"/>
+    </row>
+    <row r="764" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B764" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C764" s="5" t="n">
+        <v>898</v>
+      </c>
+      <c r="D764" s="5"/>
+      <c r="E764" s="5"/>
+    </row>
+    <row r="765" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B765" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C765" s="5" t="n">
+        <v>2985</v>
+      </c>
+      <c r="D765" s="5"/>
+      <c r="E765" s="5"/>
+    </row>
+    <row r="766" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B766" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C766" s="5" t="n">
+        <v>297</v>
+      </c>
+      <c r="D766" s="5"/>
+      <c r="E766" s="5"/>
+    </row>
+    <row r="767" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B767" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C767" s="5" t="n">
+        <v>1454</v>
+      </c>
+      <c r="D767" s="5"/>
+      <c r="E767" s="5"/>
+    </row>
+    <row r="768" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B768" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C768" s="5" t="n">
+        <v>2089</v>
+      </c>
+      <c r="D768" s="5"/>
+      <c r="E768" s="5"/>
+    </row>
+    <row r="769" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B769" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C769" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D769" s="5"/>
+      <c r="E769" s="5"/>
+    </row>
+    <row r="770" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B770" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C770" s="5" t="n">
+        <v>54</v>
+      </c>
+      <c r="D770" s="5"/>
+      <c r="E770" s="5"/>
+    </row>
+    <row r="771" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B771" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C771" s="5" t="n">
+        <v>1410</v>
+      </c>
+      <c r="D771" s="5"/>
+      <c r="E771" s="5"/>
+    </row>
+    <row r="772" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B772" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C772" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="D772" s="5"/>
+      <c r="E772" s="5"/>
+    </row>
+    <row r="773" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B773" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C773" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D773" s="5"/>
+      <c r="E773" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7769,10 +7929,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E375"/>
+  <dimension ref="A1:E390"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A356" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G353" activeCellId="0" sqref="G353"/>
+      <selection pane="topLeft" activeCell="A377" activeCellId="0" sqref="A377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12685,7 +12845,7 @@
       </c>
     </row>
     <row r="346" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A346" s="6" t="n">
+      <c r="A346" s="3" t="n">
         <v>43952</v>
       </c>
       <c r="B346" s="5" t="s">
@@ -12898,7 +13058,7 @@
       </c>
     </row>
     <row r="361" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="6" t="n">
+      <c r="A361" s="3" t="n">
         <v>43953</v>
       </c>
       <c r="B361" s="5" t="s">
@@ -13107,6 +13267,219 @@
         <v>28</v>
       </c>
       <c r="E375" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A376" s="6" t="n">
+        <v>43954</v>
+      </c>
+      <c r="B376" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C376" s="5" t="n">
+        <v>799</v>
+      </c>
+      <c r="D376" s="5" t="n">
+        <v>115</v>
+      </c>
+      <c r="E376" s="5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B377" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C377" s="5" t="n">
+        <v>284</v>
+      </c>
+      <c r="D377" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="E377" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B378" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C378" s="5" t="n">
+        <v>250</v>
+      </c>
+      <c r="D378" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="E378" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B379" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C379" s="5" t="n">
+        <v>776</v>
+      </c>
+      <c r="D379" s="5" t="n">
+        <v>123</v>
+      </c>
+      <c r="E379" s="5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B380" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C380" s="5" t="n">
+        <v>788</v>
+      </c>
+      <c r="D380" s="5" t="n">
+        <v>66</v>
+      </c>
+      <c r="E380" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B381" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C381" s="5" t="n">
+        <v>898</v>
+      </c>
+      <c r="D381" s="5" t="n">
+        <v>147</v>
+      </c>
+      <c r="E381" s="5" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B382" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C382" s="5" t="n">
+        <v>2985</v>
+      </c>
+      <c r="D382" s="5" t="n">
+        <v>526</v>
+      </c>
+      <c r="E382" s="5" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B383" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C383" s="5" t="n">
+        <v>297</v>
+      </c>
+      <c r="D383" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="E383" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B384" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C384" s="5" t="n">
+        <v>1454</v>
+      </c>
+      <c r="D384" s="5" t="n">
+        <v>233</v>
+      </c>
+      <c r="E384" s="5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B385" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C385" s="5" t="n">
+        <v>2089</v>
+      </c>
+      <c r="D385" s="5" t="n">
+        <v>269</v>
+      </c>
+      <c r="E385" s="5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B386" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C386" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D386" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E386" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B387" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C387" s="5" t="n">
+        <v>54</v>
+      </c>
+      <c r="D387" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E387" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B388" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C388" s="5" t="n">
+        <v>1410</v>
+      </c>
+      <c r="D388" s="5" t="n">
+        <v>88</v>
+      </c>
+      <c r="E388" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B389" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C389" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="D389" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E389" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="390" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B390" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C390" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D390" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E390" s="5" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>